<commit_message>
Remove Cell.richtext(), add getter RichTexts.text, add unit tests, update e2e-parse test
</commit_message>
<xml_diff>
--- a/test/e2e-parse/richtext/input.xlsx
+++ b/test/e2e-parse/richtext/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xlsx-populate\test\e2e-parse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xlsx-populate\test\e2e-parse\richtext\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F0D869-F6F8-41F3-90E1-33C9C3BB1B3F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F702562-2A85-414D-992B-1A7F1B92F710}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5424" yWindow="3288" windowWidth="22704" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7440" yWindow="3540" windowWidth="22116" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,27 +35,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">test
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF123456"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>123</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -83,6 +62,7 @@
         <sz val="20"/>
         <color theme="1"/>
         <rFont val="Aharoni"/>
+        <charset val="177"/>
       </rPr>
       <t>c</t>
     </r>
@@ -112,8 +92,96 @@
         <sz val="11"/>
         <color rgb="FF0000FF"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>123</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF123456"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">123
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF654321"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">456
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">789
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF00FF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>10
+11
+12</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="20"/>
+        <rFont val="Calibri Light"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">10
+11
+</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="20"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>12</t>
     </r>
   </si>
 </sst>
@@ -124,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,28 +249,67 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Aharoni"/>
+      <charset val="177"/>
     </font>
     <font>
       <b/>
       <i/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF123456"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF654321"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="20"/>
+      <name val="Calibri Light"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -238,9 +345,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -567,7 +673,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,31 +681,31 @@
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:5" ht="160.80000000000001" x14ac:dyDescent="0.4">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="25.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>